<commit_message>
Reference plot added to Gini vs Entropy added
</commit_message>
<xml_diff>
--- a/GINI vs ENTROPY.xlsx
+++ b/GINI vs ENTROPY.xlsx
@@ -1395,11 +1395,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="65991424"/>
-        <c:axId val="65992960"/>
+        <c:axId val="227529472"/>
+        <c:axId val="227532160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="65991424"/>
+        <c:axId val="227529472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1409,12 +1409,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65992960"/>
+        <c:crossAx val="227532160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="65992960"/>
+        <c:axId val="227532160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1425,7 +1425,1395 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65991424"/>
+        <c:crossAx val="227529472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Foglio1!$E$4:$F$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GINI ENTROPY</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Foglio1!$E$5:$E$104</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9997959391898787E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.958779716355474E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.8769513314967867E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.754310784613816E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.5908580757065612E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.11386593204775024</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.13141516171819204</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.14855626976839101</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.16528925619834711</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.18161412100806043</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.19753086419753085</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.21303948576675849</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.22813998571574332</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.2428323640444853</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.25711662075298441</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.27099275584124072</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.28446076930925418</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.2975206611570248</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.31017243138455264</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.32241607999183763</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.33425160697887968</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.34567901234567905</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.35669829609223552</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.36730945821854916</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.37751249872461995</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.38730741761044796</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.39669421487603312</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.4056728905213754</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.41424344454647483</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.42240587695133153</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.43016018773594533</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.4375063769003163</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.44444444444444448</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.45097439036832981</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.45709621467197226</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.46280991735537191</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.46811549841852879</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.47301295786144271</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.47750229568411384</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.48158351188654219</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.48525660646872776</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.48852157943067032</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.49137843077237014</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.49382716049382724</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.49586776859504134</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.49750025507601259</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.49872461993674116</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.49954086317722679</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.49994898479746958</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.49994898479746963</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.49954086317722679</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.49872461993674116</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.49750025507601264</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.49586776859504134</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.49382716049382713</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.49137843077237014</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.48852157943067032</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.4852566064687277</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.48158351188654219</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.47750229568411384</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.47301295786144265</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.46811549841852873</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.46280991735537186</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.4570962146719722</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.45097439036832976</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.44444444444444442</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.4375063769003163</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.43016018773594522</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.42240587695133147</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.41424344454647477</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.40567289052137534</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.39669421487603301</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.38730741761044785</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.37751249872461989</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.36730945821854905</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.35669829609223541</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.34567901234567899</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.33425160697887962</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.32241607999183752</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.31017243138455247</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.29752066115702475</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.28446076930925401</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.27099275584124061</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.25711662075298436</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.24283236404448513</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.22813998571574323</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.21303948576675832</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.19753086419753077</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.18161412100806021</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.16528925619834697</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.14855626976839093</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.13141516171819184</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.11386593204775014</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>9.590858075706539E-2</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>7.7543107846138021E-2</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>5.8769513314967811E-2</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>3.958779716355456E-2</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>1.9997959391898697E-2</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Foglio1!$F$5:$F$104</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.1462026915060007E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.14257333025989871</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.19590927087360493</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.24414164238829614</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.28853851369441036</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.32984607020714635</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.36855677753770649</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.40502013262424236</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.4394969869215134</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.47218938467675087</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.50325833477564574</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.53283506303422346</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.56102848634006797</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.58793037280171978</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.61361901959937082</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.63816194531400616</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.6616179061408356</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.68403843563904188</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.7054690408228711</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.72595014529437341</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.74551784281082867</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.76420450650862026</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.78203928663492495</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.79904852104426816</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.81525607663607036</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.83068363553506774</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.84535093662243654</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.85927598066096977</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.87247520548519308</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.88496363638315301</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.89675501576631456</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.90786191542636985</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.91829583405448956</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.92806728220727552</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.9371858565132074</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.94566030460064021</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.95349858197599935</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.96070790187564692</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.96729477894689453</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.97326506747513375</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.97862399475899731</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.98337619013922373</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.98752571010571022</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.99107605983822222</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.99403021147695647</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.99639061936776974</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.99815923248177385</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.99933750416888467</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.9999263993686861</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.99992639936868599</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.99933750416888456</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.99815923248177385</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.99639061936776985</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.99403021147695636</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.99107605983822222</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.98752571010571022</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.98337619013922373</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.97862399475899742</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.97326506747513364</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.96729477894689442</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.96070790187564681</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.95349858197599935</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.94566030460063999</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.93718585651320729</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.92806728220727552</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.91829583405448956</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.90786191542636985</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.89675501576631445</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.88496363638315279</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.87247520548519286</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.85927598066096977</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.84535093662243654</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.83068363553506752</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.81525607663607014</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.79904852104426793</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.78203928663492484</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.76420450650862026</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.74551784281082822</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.72595014529437352</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.70546904082287099</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.68403843563904165</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.66161790614083527</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.63816194531400583</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.61361901959937071</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.58793037280171945</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.56102848634006797</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.53283506303422312</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.50325833477564552</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.47218938467675048</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.43949698692151307</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.40502013262424225</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.3685567775377061</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.32984607020714618</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.28853851369440991</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.24414164238829569</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.19590927087360485</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.14257333025989816</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>8.1462026915059757E-2</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>REFERENCE</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Foglio1!$C$5:$C$104</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0101010101010102E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0202020202020204E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0303030303030304E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0404040404040407E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0505050505050511E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.0606060606060608E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.0707070707070718E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.0808080808080815E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.0909090909090912E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.10101010101010102</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.11111111111111112</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.12121212121212122</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.13131313131313133</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.14141414141414144</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.15151515151515152</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.16161616161616163</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.17171717171717174</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.18181818181818182</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.19191919191919193</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.20202020202020204</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.21212121212121213</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.22222222222222224</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.23232323232323235</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.24242424242424243</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.25252525252525254</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.26262626262626265</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.27272727272727276</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.28282828282828287</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.29292929292929293</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.30303030303030304</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.31313131313131315</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.32323232323232326</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.33333333333333337</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.34343434343434348</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.35353535353535359</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.36363636363636365</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.37373737373737376</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.38383838383838387</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.39393939393939398</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.40404040404040409</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.4141414141414142</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.42424242424242425</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.43434343434343436</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.44444444444444448</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.45454545454545459</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.4646464646464647</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.47474747474747481</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.48484848484848486</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.49494949494949497</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.50505050505050508</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.51515151515151525</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.5252525252525253</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.53535353535353536</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.54545454545454553</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.55555555555555558</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.56565656565656575</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.5757575757575758</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.58585858585858586</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.59595959595959602</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.60606060606060608</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.61616161616161624</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.6262626262626263</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.63636363636363646</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.64646464646464652</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.65656565656565657</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.66666666666666674</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.6767676767676768</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.68686868686868696</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.69696969696969702</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.70707070707070718</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.71717171717171724</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.72727272727272729</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.73737373737373746</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.74747474747474751</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.75757575757575768</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.76767676767676774</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.77777777777777779</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.78787878787878796</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.79797979797979801</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.80808080808080818</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.81818181818181823</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.8282828282828284</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.83838383838383845</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.84848484848484851</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.85858585858585867</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.86868686868686873</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.8787878787878789</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.88888888888888895</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.89898989898989912</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.90909090909090917</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.91919191919191923</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.92929292929292939</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.93939393939393945</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.94949494949494961</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.95959595959595967</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.96969696969696972</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.97979797979797989</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.98989898989898994</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Foglio1!$C$5:$C$104</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0101010101010102E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0202020202020204E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0303030303030304E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0404040404040407E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0505050505050511E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.0606060606060608E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.0707070707070718E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.0808080808080815E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.0909090909090912E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.10101010101010102</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.11111111111111112</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.12121212121212122</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.13131313131313133</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.14141414141414144</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.15151515151515152</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.16161616161616163</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.17171717171717174</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.18181818181818182</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.19191919191919193</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.20202020202020204</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.21212121212121213</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.22222222222222224</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.23232323232323235</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.24242424242424243</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.25252525252525254</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.26262626262626265</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.27272727272727276</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.28282828282828287</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.29292929292929293</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.30303030303030304</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.31313131313131315</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.32323232323232326</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.33333333333333337</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.34343434343434348</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.35353535353535359</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.36363636363636365</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.37373737373737376</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.38383838383838387</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.39393939393939398</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.40404040404040409</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.4141414141414142</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.42424242424242425</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.43434343434343436</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.44444444444444448</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.45454545454545459</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.4646464646464647</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.47474747474747481</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.48484848484848486</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.49494949494949497</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.50505050505050508</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.51515151515151525</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.5252525252525253</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.53535353535353536</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.54545454545454553</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.55555555555555558</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.56565656565656575</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.5757575757575758</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.58585858585858586</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.59595959595959602</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.60606060606060608</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.61616161616161624</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.6262626262626263</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.63636363636363646</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.64646464646464652</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.65656565656565657</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.66666666666666674</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.6767676767676768</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.68686868686868696</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.69696969696969702</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.70707070707070718</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.71717171717171724</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.72727272727272729</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.73737373737373746</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.74747474747474751</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.75757575757575768</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.76767676767676774</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.77777777777777779</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.78787878787878796</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.79797979797979801</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.80808080808080818</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.81818181818181823</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.8282828282828284</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.83838383838383845</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.84848484848484851</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.85858585858585867</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.86868686868686873</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.8787878787878789</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.88888888888888895</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.89898989898989912</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.90909090909090917</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.91919191919191923</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.92929292929292939</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.93939393939393945</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.94949494949494961</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.95959595959595967</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.96969696969696972</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.97979797979797989</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.98989898989898994</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="68927488"/>
+        <c:axId val="68925696"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="68927488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>ENTROPY</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="68925696"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="68925696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>GINI</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="68927488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1474,6 +2862,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>80961</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>295274</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Grafico 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1772,7 +3190,7 @@
   <dimension ref="A1:F104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>